<commit_message>
Add final version of test cases
</commit_message>
<xml_diff>
--- a/Test Cases/Test_Cases.xlsx
+++ b/Test Cases/Test_Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Home_Page" sheetId="1" r:id="rId1"/>
@@ -428,9 +428,6 @@
     <t>Verify that a user can logout from his/her account.</t>
   </si>
   <si>
-    <t>Verify that a user can recover a password.</t>
-  </si>
-  <si>
     <t>Verify that a user can modify personal information.</t>
   </si>
   <si>
@@ -753,6 +750,9 @@
 Compositions: Cotton
 Styles: Casual
 Range: 16.03 (using the right/left keys on the keyboards)</t>
+  </si>
+  <si>
+    <t>Verify that a user can retrieve a password.</t>
   </si>
 </sst>
 </file>
@@ -922,11 +922,20 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -937,9 +946,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -949,8 +955,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -961,19 +973,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1258,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,7 +1282,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -1290,10 +1290,10 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1302,17 +1302,17 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="26">
+      <c r="B3" s="12">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>186</v>
+      <c r="D3" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -1328,14 +1328,14 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -1346,17 +1346,17 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="26">
+      <c r="B5" s="12">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>186</v>
+      <c r="D5" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -1372,10 +1372,10 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="2">
         <v>2</v>
       </c>
@@ -1390,15 +1390,15 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="2">
         <v>3</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>15</v>
@@ -1408,22 +1408,22 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="26">
+      <c r="B8" s="12">
         <v>3</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>186</v>
+      <c r="E8" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -1434,10 +1434,10 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="2">
         <v>2</v>
       </c>
@@ -1452,17 +1452,17 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="26">
+      <c r="B10" s="12">
         <v>4</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>186</v>
+      <c r="E10" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -1478,10 +1478,10 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="2">
         <v>2</v>
       </c>
@@ -1496,10 +1496,10 @@
       </c>
     </row>
     <row r="12" spans="2:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="26"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="2">
         <v>3</v>
       </c>
@@ -1514,10 +1514,10 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="2">
         <v>4</v>
       </c>
@@ -1532,10 +1532,10 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="2">
         <v>5</v>
       </c>
@@ -1550,10 +1550,10 @@
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="26"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="2">
         <v>6</v>
       </c>
@@ -1568,10 +1568,10 @@
       </c>
     </row>
     <row r="16" spans="2:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="2">
         <v>7</v>
       </c>
@@ -1586,17 +1586,17 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26">
+      <c r="B17" s="12">
         <v>5</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>186</v>
+      <c r="E17" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
@@ -1612,10 +1612,10 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="2">
         <v>2</v>
       </c>
@@ -1630,10 +1630,10 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="2">
         <v>3</v>
       </c>
@@ -1648,17 +1648,17 @@
       </c>
     </row>
     <row r="20" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="26">
+      <c r="B20" s="12">
         <v>6</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>186</v>
+      <c r="E20" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
@@ -1674,10 +1674,10 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="2">
         <v>2</v>
       </c>
@@ -1692,10 +1692,10 @@
       </c>
     </row>
     <row r="22" spans="2:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="2">
         <v>3</v>
       </c>
@@ -1710,17 +1710,17 @@
       </c>
     </row>
     <row r="23" spans="2:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="26">
-        <v>7</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="12">
+        <v>7</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>186</v>
+      <c r="E23" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
@@ -1736,10 +1736,10 @@
       </c>
     </row>
     <row r="24" spans="2:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="26"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="2">
         <v>2</v>
       </c>
@@ -1755,19 +1755,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
@@ -1784,6 +1771,19 @@
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1794,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,10 +1823,10 @@
       <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1835,16 +1835,16 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="11">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="5">
@@ -1861,10 +1861,10 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="5">
         <v>2</v>
       </c>
@@ -1879,10 +1879,10 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="5">
         <v>3</v>
       </c>
@@ -1897,15 +1897,15 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="84" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>65</v>
@@ -1915,16 +1915,16 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+      <c r="B7" s="14">
         <v>2</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="5">
@@ -1941,10 +1941,10 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="5">
         <v>2</v>
       </c>
@@ -1959,10 +1959,10 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="5">
         <v>3</v>
       </c>
@@ -1977,10 +1977,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="5">
         <v>4</v>
       </c>
@@ -1995,10 +1995,10 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="84" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="5">
         <v>5</v>
       </c>
@@ -2013,16 +2013,16 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="11">
+      <c r="B12" s="14">
         <v>3</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="5">
@@ -2039,10 +2039,10 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="96" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="5">
         <v>2</v>
       </c>
@@ -2057,10 +2057,10 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="5">
         <v>3</v>
       </c>
@@ -2075,10 +2075,10 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="96" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="5">
         <v>4</v>
       </c>
@@ -2093,17 +2093,17 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="11">
+      <c r="B16" s="14">
         <v>4</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>186</v>
+      <c r="E16" s="15" t="s">
+        <v>185</v>
       </c>
       <c r="F16" s="5">
         <v>1</v>
@@ -2119,10 +2119,10 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="96" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="5">
         <v>2</v>
       </c>
@@ -2137,10 +2137,10 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
       <c r="F18" s="5">
         <v>3</v>
       </c>
@@ -2155,10 +2155,10 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="5">
         <v>4</v>
       </c>
@@ -2173,10 +2173,10 @@
       </c>
     </row>
     <row r="20" spans="2:9" ht="84" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="5">
         <v>5</v>
       </c>
@@ -2191,10 +2191,10 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="5">
         <v>6</v>
       </c>
@@ -2209,16 +2209,16 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="11">
+      <c r="B22" s="14">
         <v>5</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="5">
@@ -2235,10 +2235,10 @@
       </c>
     </row>
     <row r="23" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="5">
         <v>2</v>
       </c>
@@ -2253,10 +2253,10 @@
       </c>
     </row>
     <row r="24" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="5">
         <v>3</v>
       </c>
@@ -2271,10 +2271,10 @@
       </c>
     </row>
     <row r="25" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="5">
         <v>4</v>
       </c>
@@ -2289,10 +2289,10 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="5">
         <v>5</v>
       </c>
@@ -2307,10 +2307,10 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="5">
         <v>6</v>
       </c>
@@ -2325,16 +2325,16 @@
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="11">
+      <c r="B28" s="14">
         <v>6</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="5">
@@ -2351,10 +2351,10 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
       <c r="F29" s="5">
         <v>2</v>
       </c>
@@ -2369,10 +2369,10 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
       <c r="F30" s="5">
         <v>3</v>
       </c>
@@ -2387,10 +2387,10 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
       <c r="F31" s="5">
         <v>4</v>
       </c>
@@ -2405,10 +2405,10 @@
       </c>
     </row>
     <row r="32" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
       <c r="F32" s="5">
         <v>5</v>
       </c>
@@ -2424,15 +2424,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="E22:E27"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="C16:C21"/>
-    <mergeCell ref="D16:D21"/>
-    <mergeCell ref="E16:E21"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="C28:C32"/>
     <mergeCell ref="D28:D32"/>
@@ -2449,6 +2440,15 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="E12:E15"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="D16:D21"/>
+    <mergeCell ref="E16:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2458,8 +2458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,10 +2486,10 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2497,18 +2497,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B3" s="11">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>185</v>
+      <c r="E3" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
@@ -2524,10 +2524,10 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="5">
         <v>2</v>
       </c>
@@ -2542,10 +2542,10 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="5">
         <v>3</v>
       </c>
@@ -2560,215 +2560,215 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="I6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="5">
         <v>5</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>121</v>
-      </c>
       <c r="I7" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="5">
         <v>6</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="5">
+        <v>7</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="5">
-        <v>7</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>125</v>
-      </c>
       <c r="I9" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="5">
         <v>8</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>127</v>
-      </c>
       <c r="I10" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="5">
         <v>9</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>129</v>
-      </c>
       <c r="I11" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="5">
         <v>10</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>131</v>
-      </c>
       <c r="I12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="5">
         <v>11</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="5">
         <v>12</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="5">
         <v>13</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="I15" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="5">
         <v>14</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>139</v>
-      </c>
       <c r="I16" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B17" s="11">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="14">
         <v>2</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>187</v>
+      <c r="E17" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="F17" s="5">
         <v>1</v>
@@ -2784,10 +2784,10 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
       <c r="F18" s="5">
         <v>2</v>
       </c>
@@ -2802,10 +2802,10 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="5">
         <v>3</v>
       </c>
@@ -2820,197 +2820,197 @@
       </c>
     </row>
     <row r="20" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="5">
         <v>4</v>
       </c>
       <c r="G20" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="I20" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="5">
         <v>5</v>
       </c>
       <c r="G21" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>121</v>
-      </c>
       <c r="I21" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="5">
         <v>6</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="I22" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="5">
+        <v>7</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="5">
-        <v>7</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>125</v>
-      </c>
       <c r="I23" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="5">
         <v>8</v>
       </c>
       <c r="G24" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>141</v>
-      </c>
       <c r="I24" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="5">
         <v>9</v>
       </c>
       <c r="G25" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="I25" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="5">
         <v>10</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="5">
         <v>11</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
       <c r="F28" s="5">
         <v>12</v>
       </c>
       <c r="G28" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="I28" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
       <c r="F29" s="5">
         <v>13</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>139</v>
-      </c>
       <c r="I29" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B30" s="11">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="14">
         <v>3</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>185</v>
+      <c r="E30" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="F30" s="5">
         <v>1</v>
@@ -3026,10 +3026,10 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
       <c r="F31" s="5">
         <v>2</v>
       </c>
@@ -3044,10 +3044,10 @@
       </c>
     </row>
     <row r="32" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
       <c r="F32" s="5">
         <v>3</v>
       </c>
@@ -3062,89 +3062,89 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
       <c r="F33" s="5">
         <v>4</v>
       </c>
       <c r="G33" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="I33" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
       <c r="F34" s="5">
         <v>5</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
       <c r="F35" s="5">
         <v>6</v>
       </c>
       <c r="G35" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="I35" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
       <c r="F36" s="5">
         <v>7</v>
       </c>
       <c r="G36" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>146</v>
-      </c>
       <c r="I36" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B37" s="11">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="14">
         <v>4</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="12" t="s">
-        <v>185</v>
+      <c r="E37" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="F37" s="5">
         <v>1</v>
@@ -3160,10 +3160,10 @@
       </c>
     </row>
     <row r="38" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
       <c r="F38" s="5">
         <v>2</v>
       </c>
@@ -3178,10 +3178,10 @@
       </c>
     </row>
     <row r="39" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
       <c r="F39" s="5">
         <v>3</v>
       </c>
@@ -3196,89 +3196,89 @@
       </c>
     </row>
     <row r="40" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
       <c r="F40" s="5">
         <v>4</v>
       </c>
       <c r="G40" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H40" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="I40" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
       <c r="F41" s="5">
         <v>5</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
       <c r="F42" s="5">
         <v>6</v>
       </c>
       <c r="G42" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="I42" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="5">
+        <v>7</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="I42" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="5">
-        <v>7</v>
-      </c>
-      <c r="G43" s="6" t="s">
+      <c r="H43" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>150</v>
-      </c>
       <c r="I43" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B44" s="11">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="14">
         <v>5</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="12" t="s">
-        <v>185</v>
+      <c r="E44" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="F44" s="5">
         <v>1</v>
@@ -3294,10 +3294,10 @@
       </c>
     </row>
     <row r="45" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
       <c r="F45" s="5">
         <v>2</v>
       </c>
@@ -3312,10 +3312,10 @@
       </c>
     </row>
     <row r="46" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
       <c r="F46" s="5">
         <v>3</v>
       </c>
@@ -3330,198 +3330,198 @@
       </c>
     </row>
     <row r="47" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
       <c r="F47" s="5">
         <v>4</v>
       </c>
       <c r="G47" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H47" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H47" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="I47" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="B48" s="11"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
       <c r="F48" s="5">
         <v>5</v>
       </c>
       <c r="G48" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H48" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H48" s="6" t="s">
-        <v>121</v>
-      </c>
       <c r="I48" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B49" s="11"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
       <c r="F49" s="5">
         <v>6</v>
       </c>
       <c r="G49" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H49" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H49" s="6" t="s">
+      <c r="I49" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B50" s="14"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="5">
+        <v>7</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="I49" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B50" s="11"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="5">
-        <v>7</v>
-      </c>
-      <c r="G50" s="6" t="s">
+      <c r="H50" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H50" s="6" t="s">
-        <v>125</v>
-      </c>
       <c r="I50" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
       <c r="F51" s="5">
         <v>8</v>
       </c>
       <c r="G51" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="H51" s="6" t="s">
-        <v>141</v>
-      </c>
       <c r="I51" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
       <c r="F52" s="5">
         <v>9</v>
       </c>
       <c r="G52" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="H52" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="I52" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
       <c r="F53" s="5">
         <v>10</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="54" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
       <c r="F54" s="5">
         <v>11</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B55" s="11"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
       <c r="F55" s="5">
         <v>12</v>
       </c>
       <c r="G55" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H55" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="H55" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="I55" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B56" s="11"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
       <c r="F56" s="5">
         <v>13</v>
       </c>
       <c r="G56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="H56" s="6" t="s">
-        <v>139</v>
-      </c>
       <c r="I56" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="11"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
       <c r="F57" s="5">
         <v>14</v>
       </c>
       <c r="G57" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H57" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="I57" s="6" t="s">
         <v>7</v>
@@ -3529,6 +3529,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E37:E43"/>
+    <mergeCell ref="B30:B36"/>
+    <mergeCell ref="C30:C36"/>
+    <mergeCell ref="D30:D36"/>
+    <mergeCell ref="E30:E36"/>
     <mergeCell ref="B44:B57"/>
     <mergeCell ref="C44:C57"/>
     <mergeCell ref="D44:D57"/>
@@ -3545,11 +3550,6 @@
     <mergeCell ref="B37:B43"/>
     <mergeCell ref="C37:C43"/>
     <mergeCell ref="D37:D43"/>
-    <mergeCell ref="E37:E43"/>
-    <mergeCell ref="B30:B36"/>
-    <mergeCell ref="C30:C36"/>
-    <mergeCell ref="D30:D36"/>
-    <mergeCell ref="E30:E36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3559,8 +3559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D7"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3588,10 +3588,10 @@
       <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="8" t="s">
         <v>2</v>
       </c>
@@ -3600,17 +3600,17 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="11">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>185</v>
+      <c r="E3" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
@@ -3626,89 +3626,89 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="5">
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="5">
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>156</v>
-      </c>
       <c r="I5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="216" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="5">
         <v>5</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>159</v>
-      </c>
       <c r="I7" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="11">
+      <c r="B8" s="14">
         <v>2</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>187</v>
+      <c r="E8" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="F8" s="5">
         <v>1</v>
@@ -3724,89 +3724,89 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="5">
         <v>2</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="I9" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="5">
         <v>3</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="I10" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="5">
         <v>4</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>163</v>
-      </c>
       <c r="I11" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="5">
         <v>5</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="11">
+      <c r="B13" s="14">
         <v>3</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>187</v>
+      <c r="E13" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="F13" s="5">
         <v>1</v>
@@ -3822,107 +3822,107 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="5">
         <v>2</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="I14" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="5">
         <v>3</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="I15" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="5">
         <v>4</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>163</v>
-      </c>
       <c r="I16" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="5">
         <v>5</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
       <c r="F18" s="5">
         <v>6</v>
       </c>
       <c r="G18" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="I18" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="11">
+      <c r="B19" s="14">
         <v>4</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>187</v>
+      <c r="D19" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="F19" s="5">
         <v>1</v>
@@ -3938,107 +3938,107 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="5">
         <v>2</v>
       </c>
       <c r="G20" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="I20" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="5">
         <v>3</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="5">
         <v>4</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>169</v>
-      </c>
       <c r="I22" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="5">
         <v>5</v>
       </c>
       <c r="G23" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>171</v>
-      </c>
       <c r="I23" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="5">
         <v>6</v>
       </c>
       <c r="G24" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>173</v>
-      </c>
       <c r="I24" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="11">
+      <c r="B25" s="14">
         <v>5</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>187</v>
+      <c r="D25" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="F25" s="5">
         <v>1</v>
@@ -4054,125 +4054,125 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
       <c r="F26" s="5">
         <v>2</v>
       </c>
       <c r="G26" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="I26" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
       <c r="F27" s="5">
         <v>3</v>
       </c>
       <c r="G27" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="I27" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
       <c r="F28" s="5">
         <v>4</v>
       </c>
       <c r="G28" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>163</v>
-      </c>
       <c r="I28" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="84" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
       <c r="F29" s="5">
         <v>5</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="204" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
       <c r="F30" s="5">
         <v>6</v>
       </c>
       <c r="G30" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="I30" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="5">
+        <v>7</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="I30" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="5">
-        <v>7</v>
-      </c>
-      <c r="G31" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>178</v>
-      </c>
       <c r="I31" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="15">
+      <c r="B32" s="17">
         <v>6</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>187</v>
+      <c r="D32" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>186</v>
       </c>
       <c r="F32" s="5">
         <v>1</v>
@@ -4188,89 +4188,89 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="16"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
       <c r="F33" s="5">
         <v>2</v>
       </c>
       <c r="G33" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="I33" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B34" s="16"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
       <c r="F34" s="5">
         <v>3</v>
       </c>
       <c r="G34" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="I34" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="16"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="5">
         <v>4</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B36" s="17"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
       <c r="F36" s="5">
         <v>5</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="I36" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="I36" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="19">
-        <v>7</v>
-      </c>
-      <c r="C37" s="22" t="s">
+      <c r="B37" s="23">
+        <v>7</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>187</v>
+      <c r="D37" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>186</v>
       </c>
       <c r="F37" s="5">
         <v>1</v>
@@ -4281,128 +4281,129 @@
       <c r="H37" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I37" s="18" t="s">
+      <c r="I37" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="20"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
       <c r="F38" s="5">
         <v>2</v>
       </c>
       <c r="G38" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="I38" s="18" t="s">
+      <c r="I38" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="B39" s="20"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
       <c r="F39" s="5">
         <v>3</v>
       </c>
       <c r="G39" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="I39" s="18" t="s">
+      <c r="I39" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="24" x14ac:dyDescent="0.25">
-      <c r="B40" s="20"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
       <c r="F40" s="5">
         <v>4</v>
       </c>
       <c r="G40" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="H40" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="I40" s="18" t="s">
+      <c r="I40" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="84" x14ac:dyDescent="0.25">
-      <c r="B41" s="20"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
       <c r="F41" s="5">
         <v>5</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="I41" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B42" s="20"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
       <c r="F42" s="5">
         <v>6</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="G42" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H42" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="I42" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="25"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="5">
+        <v>7</v>
+      </c>
+      <c r="G43" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="I42" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="21"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="5">
-        <v>7</v>
-      </c>
-      <c r="G43" s="18" t="s">
+      <c r="H43" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="H43" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="I43" s="18" t="s">
+      <c r="I43" s="9" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="C37:C43"/>
-    <mergeCell ref="D37:D43"/>
-    <mergeCell ref="E37:E43"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="E3:E7"/>
     <mergeCell ref="B25:B31"/>
     <mergeCell ref="C25:C31"/>
     <mergeCell ref="D25:D31"/>
@@ -4415,15 +4416,14 @@
     <mergeCell ref="C19:C24"/>
     <mergeCell ref="D19:D24"/>
     <mergeCell ref="E19:E24"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="C37:C43"/>
+    <mergeCell ref="D37:D43"/>
+    <mergeCell ref="E37:E43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>